<commit_message>
W zasadzie prawie koniec
</commit_message>
<xml_diff>
--- a/lab08/references/T1_latex_table_export.xlsx
+++ b/lab08/references/T1_latex_table_export.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">l.p</t>
   </si>
@@ -47,9 +47,6 @@
   <si>
     <t xml:space="preserve">sqrt</t>
   </si>
-  <si>
-    <t xml:space="preserve">liest</t>
-  </si>
 </sst>
 </file>
 
@@ -60,7 +57,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -83,16 +80,139 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -100,8 +220,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -125,6 +260,54 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -140,14 +323,90 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -156,28 +415,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="8" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="33.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="8.57"/>
   </cols>
   <sheetData>
@@ -203,11 +462,8 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -235,11 +491,8 @@
         <f aca="false">SQRT((C2/B2)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0176331566136861</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <f aca="false">SQRT(ABS(D2))</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
         <v>0</v>
       </c>
     </row>
@@ -268,12 +521,9 @@
         <f aca="false">SQRT((C3/B3)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0197388927170629</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <f aca="false">SQRT(ABS(D3))</f>
         <v>0.109544511501033</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>-0.165707774818225</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -301,12 +551,9 @@
         <f aca="false">SQRT((C4/B4)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0203090076479504</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <f aca="false">SQRT(ABS(D4))</f>
         <v>0.134164078649987</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>-0.248561662227338</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,12 +581,9 @@
         <f aca="false">SQRT((C5/B5)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0209474924373951</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <f aca="false">SQRT(ABS(D5))</f>
         <v>0.144913767461894</v>
-      </c>
-      <c r="K5" s="0" t="n">
-        <v>-0.289988605931894</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,12 +611,9 @@
         <f aca="false">SQRT((C6/B6)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0224779524148558</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <f aca="false">SQRT(ABS(D6))</f>
         <v>0.173205080756888</v>
-      </c>
-      <c r="K6" s="0" t="n">
-        <v>-0.414269437045564</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -400,12 +641,9 @@
         <f aca="false">SQRT((C7/B7)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0244575640531662</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <f aca="false">SQRT(ABS(D7))</f>
         <v>0.194935886896179</v>
-      </c>
-      <c r="K7" s="0" t="n">
-        <v>-0.52474128692438</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -433,12 +671,9 @@
         <f aca="false">SQRT((C8/B8)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0270868122635056</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <f aca="false">SQRT(ABS(D8))</f>
         <v>0.212132034355964</v>
-      </c>
-      <c r="K8" s="0" t="n">
-        <v>-0.621404155568345</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,12 +701,9 @@
         <f aca="false">SQRT((C9/B9)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0287415299857819</v>
       </c>
-      <c r="I9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <f aca="false">SQRT(ABS(D9))</f>
         <v>0.234520787991171</v>
-      </c>
-      <c r="K9" s="0" t="n">
-        <v>-0.759493967916866</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -499,12 +731,9 @@
         <f aca="false">SQRT((C10/B10)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0330469851051302</v>
       </c>
-      <c r="I10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <f aca="false">SQRT(ABS(D10))</f>
         <v>0.254950975679639</v>
-      </c>
-      <c r="K10" s="0" t="n">
-        <v>-0.897583780265387</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -532,12 +761,9 @@
         <f aca="false">SQRT((C11/B11)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0358998250610602</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <f aca="false">SQRT(ABS(D11))</f>
         <v>0.273861278752583</v>
-      </c>
-      <c r="K11" s="0" t="n">
-        <v>-1.03567359261391</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,12 +791,9 @@
         <f aca="false">SQRT((C12/B12)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0438896051407931</v>
       </c>
-      <c r="I12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <f aca="false">SQRT(ABS(D12))</f>
         <v>0.298328677803526</v>
-      </c>
-      <c r="K12" s="0" t="n">
-        <v>-1.22899932990184</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,12 +821,9 @@
         <f aca="false">SQRT((C13/B13)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0496828871559356</v>
       </c>
-      <c r="I13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <f aca="false">SQRT(ABS(D13))</f>
         <v>0.311448230047949</v>
-      </c>
-      <c r="K13" s="0" t="n">
-        <v>-1.33947117978066</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -631,12 +851,9 @@
         <f aca="false">SQRT((C14/B14)^2+(-$C$2/$B$2)^2)</f>
         <v>0.0574770585036287</v>
       </c>
-      <c r="I14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <f aca="false">SQRT(ABS(D14))</f>
         <v>0.327108544675923</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>-1.47756099212918</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>